<commit_message>
Update output layout in outputLayout.xlsx
</commit_message>
<xml_diff>
--- a/outputLayout.xlsx
+++ b/outputLayout.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcte\OneDrive\Desktop\tmp\20250320\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcte\OneDrive\Desktop\tmp\20250320\tmpCode\my-20250319_web2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D77D05-334B-461C-AEE9-22ACF12A35E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110D8422-8F84-4C08-B9BB-4AA556F95A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
   </bookViews>
   <sheets>
     <sheet name="20_Properties of Circles" sheetId="1" r:id="rId1"/>
-    <sheet name="21_Properties of Tangent to Cir" sheetId="2" r:id="rId2"/>
+    <sheet name="21_Prop of Tangent to Circle" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,9 +90,6 @@
     <t>DSE19PII_Q38</t>
   </si>
   <si>
-    <t>21_Properties of Tangent to Cir</t>
-  </si>
-  <si>
     <t>DSE17PII_Q40</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Question Code</t>
+  </si>
+  <si>
+    <t>21_Prop of Tangent to Circle</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -520,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -660,18 +660,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FBEF4C-F3BD-4B0D-BD21-8FAD9730D529}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,7 +685,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +725,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +733,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,7 +749,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -759,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -767,7 +765,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add class filtering functionality in script.js and styles.css
</commit_message>
<xml_diff>
--- a/outputLayout.xlsx
+++ b/outputLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcte\OneDrive\Desktop\tmp\20250320\tmpCode\my-20250319_web2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110D8422-8F84-4C08-B9BB-4AA556F95A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB211EAE-5B88-4923-9C34-AE6CEA56E03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
   </bookViews>
   <sheets>
     <sheet name="20_Properties of Circles" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
-  <si>
-    <t>20_Properties of Circles</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>DSE15PII_Q21</t>
   </si>
@@ -130,9 +127,6 @@
   </si>
   <si>
     <t>Question Code</t>
-  </si>
-  <si>
-    <t>21_Prop of Tangent to Circle</t>
   </si>
 </sst>
 </file>
@@ -506,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,11 +510,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1">
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -528,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -536,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -544,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -552,7 +546,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -560,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -568,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -576,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -584,7 +578,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -592,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -600,7 +594,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -608,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -616,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -624,7 +618,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -632,7 +626,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -640,7 +634,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -648,7 +642,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -660,16 +654,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FBEF4C-F3BD-4B0D-BD21-8FAD9730D529}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>31</v>
+      <c r="A1">
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,7 +697,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -709,7 +705,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -717,7 +713,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -733,7 +729,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -741,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -749,7 +745,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -757,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -765,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -773,7 +769,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor class extraction logic in script.js to derive class from student name and improve class option sorting
</commit_message>
<xml_diff>
--- a/outputLayout.xlsx
+++ b/outputLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcte\OneDrive\Desktop\tmp\20250320\tmpCode\my-20250319_web2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB211EAE-5B88-4923-9C34-AE6CEA56E03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1B9C7-20CB-424D-BB63-C8FF8E8C66E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
+    <workbookView xWindow="10572" yWindow="3264" windowWidth="10488" windowHeight="8988" firstSheet="1" activeTab="1" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
   </bookViews>
   <sheets>
     <sheet name="20_Properties of Circles" sheetId="1" r:id="rId1"/>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FBEF4C-F3BD-4B0D-BD21-8FAD9730D529}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,7 +686,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Update output layout in outputLayout.xlsx for improved data presentation
</commit_message>
<xml_diff>
--- a/outputLayout.xlsx
+++ b/outputLayout.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcte\OneDrive\Desktop\tmp\20250320\tmpCode\my-20250319_web2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcht\Desktop\tmp\20250321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1B9C7-20CB-424D-BB63-C8FF8E8C66E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBD1CED-D6CF-4203-B38A-CFE5AB232136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10572" yWindow="3264" windowWidth="10488" windowHeight="8988" firstSheet="1" activeTab="1" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="20_Properties of Circles" sheetId="1" r:id="rId1"/>
-    <sheet name="21_Prop of Tangent to Circle" sheetId="2" r:id="rId2"/>
+    <sheet name="01_Change of Subjects" sheetId="3" r:id="rId1"/>
+    <sheet name="20_Properties of Circles" sheetId="1" r:id="rId2"/>
+    <sheet name="21_Prop of Tangent to Circle" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>DSE15PII_Q21</t>
   </si>
@@ -127,18 +128,61 @@
   </si>
   <si>
     <t>Question Code</t>
+  </si>
+  <si>
+    <t>DSE24PII_Q03</t>
+  </si>
+  <si>
+    <t>DSE21PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE20PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE13PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE16PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE22PII_Q05</t>
+  </si>
+  <si>
+    <t>DSE18PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE23PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE19PII_Q05</t>
+  </si>
+  <si>
+    <t>DSE17PII_Q03</t>
+  </si>
+  <si>
+    <t>DSEPPPII_Q02</t>
+  </si>
+  <si>
+    <t>DSESPPII_Q02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -166,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -182,7 +226,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,170 +541,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293DADDA-523F-4627-8CBE-9A308B924E03}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FBEF4C-F3BD-4B0D-BD21-8FAD9730D529}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>21</v>
       </c>
@@ -668,7 +833,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -676,7 +841,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -684,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -692,7 +857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -700,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -708,7 +873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -716,7 +881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -724,7 +889,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -732,7 +897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -740,7 +905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -748,7 +913,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -756,7 +921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -764,7 +929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -773,6 +938,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update output layout in outputLayout.xlsx for enhanced data presentation
</commit_message>
<xml_diff>
--- a/outputLayout.xlsx
+++ b/outputLayout.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\htcht\Desktop\tmp\20250321\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teacher\Desktop\tmp\20250321\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBD1CED-D6CF-4203-B38A-CFE5AB232136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD4B9ED-0057-4A7D-9D3C-367D20135491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{FE39667E-84F3-4DA3-BA14-93FFA1D9EAF0}"/>
   </bookViews>
   <sheets>
     <sheet name="01_Change of Subjects" sheetId="3" r:id="rId1"/>
-    <sheet name="20_Properties of Circles" sheetId="1" r:id="rId2"/>
-    <sheet name="21_Prop of Tangent to Circle" sheetId="2" r:id="rId3"/>
+    <sheet name="02_Law of Indices" sheetId="4" r:id="rId2"/>
+    <sheet name="20_Properties of Circles" sheetId="1" r:id="rId3"/>
+    <sheet name="21_Prop of Tangent to Circle" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>DSE15PII_Q21</t>
   </si>
@@ -164,6 +165,48 @@
   </si>
   <si>
     <t>DSESPPII_Q02</t>
+  </si>
+  <si>
+    <t>DSE12PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE14PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE15PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE19PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE22PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE24PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE20PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE21PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE23PII_Q03</t>
+  </si>
+  <si>
+    <t>DSE17PII_Q02</t>
+  </si>
+  <si>
+    <t>DSE18PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE13PII_Q01</t>
+  </si>
+  <si>
+    <t>DSE16PII_Q01</t>
+  </si>
+  <si>
+    <t>DSESPPII_Q01</t>
   </si>
 </sst>
 </file>
@@ -210,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -226,7 +269,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -544,13 +587,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293DADDA-523F-4627-8CBE-9A308B924E03}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -558,7 +601,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -566,7 +609,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -574,7 +617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -582,7 +625,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -590,7 +633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -598,7 +641,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -606,7 +649,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -614,7 +657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -622,7 +665,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -630,7 +673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -638,7 +681,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -646,7 +689,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -661,6 +704,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEA36F4-9052-45DA-9D1E-6917CCFA1B56}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B04157-5176-4757-B397-5C6D792D534C}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -668,12 +847,12 @@
       <selection sqref="A1:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>20</v>
       </c>
@@ -681,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -689,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -697,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -705,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -713,7 +892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -721,7 +900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -729,7 +908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -737,7 +916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -745,7 +924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -753,7 +932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -761,7 +940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -769,7 +948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -777,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -785,7 +964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -793,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -801,7 +980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -815,7 +994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FBEF4C-F3BD-4B0D-BD21-8FAD9730D529}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -823,9 +1002,9 @@
       <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>21</v>
       </c>
@@ -833,7 +1012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -841,7 +1020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -849,7 +1028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -857,7 +1036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -865,7 +1044,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -873,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -881,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -889,7 +1068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -897,7 +1076,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -905,7 +1084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -913,7 +1092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -921,7 +1100,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -929,7 +1108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>

</xml_diff>